<commit_message>
update some camera info
</commit_message>
<xml_diff>
--- a/Data_raw/Camera_locs.xlsx
+++ b/Data_raw/Camera_locs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Documents/University/PhD/Data/Gosforth_mammals/Data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479E0918-D74F-DF4C-8551-C719DF4A0504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC4BC51-19E2-8B4B-97A7-0E5EB6C7AE2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="17540" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="17500" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Point_ID</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>064</t>
+  </si>
+  <si>
+    <t>Date_off</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>001</t>
   </si>
 </sst>
 </file>
@@ -497,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DBF150-3A85-F348-B5D6-0CDB72BD1D6E}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +520,7 @@
     <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,16 +537,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -550,11 +565,12 @@
       <c r="E2" s="2">
         <v>44069</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -570,11 +586,12 @@
       <c r="E3" s="2">
         <v>44069</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3" s="2"/>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -590,11 +607,12 @@
       <c r="E4" s="2">
         <v>44069</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -610,11 +628,12 @@
       <c r="E5" s="2">
         <v>44069</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -630,11 +649,12 @@
       <c r="E6" s="2">
         <v>44069</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -650,11 +670,12 @@
       <c r="E7" s="2">
         <v>44074</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -670,11 +691,12 @@
       <c r="E8" s="2">
         <v>44074</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -690,11 +712,12 @@
       <c r="E9" s="2">
         <v>44074</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -710,11 +733,12 @@
       <c r="E10" s="2">
         <v>44075</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -730,11 +754,12 @@
       <c r="E11" s="2">
         <v>44075</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -750,11 +775,12 @@
       <c r="E12" s="2">
         <v>44076</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -770,11 +796,12 @@
       <c r="E13" s="2">
         <v>44076</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -790,42 +817,142 @@
       <c r="E14" s="2">
         <v>44076</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2">
         <v>44077</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2">
+        <v>44122</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="2">
         <v>44077</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G16" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="2">
+        <v>44092</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44092</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44258</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2">
+        <v>44092</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44258</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44092</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44258</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing point 5 info
</commit_message>
<xml_diff>
--- a/Data_raw/Camera_locs.xlsx
+++ b/Data_raw/Camera_locs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Gosforth_mammals/Data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB8C6BA-C410-C844-8717-E250427C921A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7EB8C6BA-C410-C844-8717-E250427C921A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FD091D01-3531-1D4D-8E78-9A492289B217}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="17500" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="16620" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -663,7 +663,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J6">
         <v>10.5</v>

</xml_diff>

<commit_message>
ok the data is ok
</commit_message>
<xml_diff>
--- a/Data_raw/Camera_locs.xlsx
+++ b/Data_raw/Camera_locs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/Gosforth_mammals/Data_raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabraunholtz/Library/Mobile Documents/com~apple~CloudDocs/Documents/University/PhD/Data/Gosforth_mammals/Data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7EB8C6BA-C410-C844-8717-E250427C921A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FD091D01-3531-1D4D-8E78-9A492289B217}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F1D91-999F-B143-9D5E-C28B3C4B9727}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="16620" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16620" xr2:uid="{BDCD2837-C9A3-764C-AD67-E7F447FA836A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
   <si>
     <t>Point_ID</t>
   </si>
@@ -47,9 +47,6 @@
     <t>SD_card</t>
   </si>
   <si>
-    <t>Date_on</t>
-  </si>
-  <si>
     <t>Tree_sp</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>064</t>
   </si>
   <si>
-    <t>Date_off</t>
-  </si>
-  <si>
     <t>025</t>
   </si>
   <si>
@@ -162,6 +156,18 @@
   </si>
   <si>
     <t>Tree_connect</t>
+  </si>
+  <si>
+    <t>Date_first_image</t>
+  </si>
+  <si>
+    <t>Date_last_image</t>
+  </si>
+  <si>
+    <t>Date_out</t>
+  </si>
+  <si>
+    <t>Date_in</t>
   </si>
 </sst>
 </file>
@@ -197,10 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DBF150-3A85-F348-B5D6-0CDB72BD1D6E}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,7 +533,7 @@
     <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,347 +547,457 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2">
         <v>44069</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>44069</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F3" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G3" s="2">
+        <v>44069</v>
+      </c>
+      <c r="H3" s="2">
+        <v>44123</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="2">
         <v>44069</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F4" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G4" s="2">
+        <v>44069</v>
+      </c>
+      <c r="H4" s="2">
+        <v>44069</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>44069</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F5" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G5" s="2">
+        <v>44069</v>
+      </c>
+      <c r="H5" s="2">
+        <v>44050</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>44069</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6">
+      <c r="F6" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G6" s="2">
+        <v>42741</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42789</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6">
         <v>10.5</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>44074</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
         <v>44074</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="2">
         <v>44074</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F9" s="3">
+        <v>44124</v>
+      </c>
+      <c r="G9" s="2">
+        <v>44074</v>
+      </c>
+      <c r="H9" s="2">
+        <v>44124</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="2">
         <v>44075</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>44075</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E12" s="2">
         <v>44076</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2">
         <v>44076</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>44124</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44076</v>
+      </c>
+      <c r="H13" s="2">
+        <v>44112</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>14</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E14" s="2">
         <v>44076</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2">
         <v>44077</v>
       </c>
       <c r="F15" s="2">
-        <v>44122</v>
-      </c>
-      <c r="G15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15">
+        <v>44123</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44077</v>
+      </c>
+      <c r="H15" s="2">
+        <v>44123</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15">
         <v>12</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2">
         <v>44077</v>
@@ -888,49 +1005,69 @@
       <c r="F16" s="2">
         <v>44123</v>
       </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16">
+      <c r="G16" s="2">
+        <v>44077</v>
+      </c>
+      <c r="H16" s="2">
+        <v>44121</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16">
         <v>8.5</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2">
         <v>44092</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
+        <v>44123</v>
+      </c>
+      <c r="G17" s="2">
+        <v>44092</v>
+      </c>
+      <c r="H17" s="2">
+        <v>44123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2">
         <v>44092</v>
@@ -938,22 +1075,34 @@
       <c r="F18" s="2">
         <v>44258</v>
       </c>
-      <c r="G18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="2">
+        <v>44092</v>
+      </c>
+      <c r="H18" s="2">
+        <v>44237</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2">
         <v>44092</v>
@@ -961,19 +1110,34 @@
       <c r="F19" s="2">
         <v>44258</v>
       </c>
-      <c r="G19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="2">
+        <v>44092</v>
+      </c>
+      <c r="H19" s="2">
+        <v>44258</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E20" s="2">
         <v>44092</v>
@@ -981,8 +1145,20 @@
       <c r="F20" s="2">
         <v>44258</v>
       </c>
-      <c r="G20" t="s">
-        <v>17</v>
+      <c r="G20" s="2">
+        <v>44092</v>
+      </c>
+      <c r="H20" s="2">
+        <v>44258</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>